<commit_message>
Add evidence for A1-A6 tasks (stage-1)
</commit_message>
<xml_diff>
--- a/ibrahimarslann59/evidence.xlsx
+++ b/ibrahimarslann59/evidence.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="45">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -117,34 +117,58 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class id you issued</t>
+    <t xml:space="preserve">13E408B5F64EE5E3F15D3F7A70EE702CEB92282EAA70A016D894989AFE43AE8D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">belloma</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">nft id you minted</t>
+    <t xml:space="preserve">428F114E0355F96F8360288B4E788D1BCF6BD3FDAF6BD334D5E6C62B2D18BCDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bellomanft1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">762D564A59618C07C18A511CCC0FE996A48097BA1ACCEA371F4991E743E861FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bellomanft2</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on dest chain</t>
+    <t xml:space="preserve">15435648EC5DF4F95159688A71F9B9A19BACDBFAD60099F333865853AB31C402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juno1w2r28luz5ntl4pd8krrtg5j6eyyljc3u7kpw02kj03ya4lk8jjms9ygjuc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCA2E37A3518F3891C4AA2D67B7E53B738AE9E9AC7CBFF6AAEE96C13BD223E70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/C49AC2E4229E7945F9E372B95532474F0625F0DAD0FEA246B1EBC3985C7E5DD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gon-flixnet-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3AAB3B3A4B3B0F59901F0891E003C0030DFCFA8710B538A500471D6570E8F1EA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1BBCC07A7767A20C0D7AC1F26899A004AAD06DDEB6A539082A02677BB0B7784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -385,7 +409,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.86"/>
@@ -491,7 +515,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -507,10 +531,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -535,7 +559,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -551,10 +575,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +603,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -595,10 +619,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +647,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -639,10 +663,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -667,7 +691,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -678,25 +702,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +745,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -732,25 +756,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +799,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -786,25 +810,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -829,7 +853,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -840,25 +864,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +907,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -894,25 +918,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -937,7 +961,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -948,25 +972,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -988,53 +1012,53 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1045,25 +1069,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1088,7 +1112,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1099,25 +1123,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1142,7 +1166,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1154,12 +1178,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1208,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1196,12 +1220,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1250,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1238,12 +1262,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1268,7 +1292,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1280,12 +1304,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1304,13 +1328,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1329,13 +1353,24 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1357,10 +1392,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1378,21 +1413,21 @@
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1414,10 +1449,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1435,21 +1470,21 @@
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1471,10 +1506,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1492,21 +1527,21 @@
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1528,10 +1563,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
@@ -1550,21 +1585,21 @@
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1589,7 +1624,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1605,10 +1640,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1668,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1649,10 +1684,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>